<commit_message>
just open source things
</commit_message>
<xml_diff>
--- a/20170430-mnpollv3-senators/builds/development/data/maindata.xlsx
+++ b/20170430-mnpollv3-senators/builds/development/data/maindata.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3157" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3166" uniqueCount="108">
   <si>
     <t>year</t>
   </si>
@@ -322,12 +322,36 @@
   <si>
     <t>Poll conducted by Mason-Dixon Polling and Strategy on behalf of the Star Tribune</t>
   </si>
+  <si>
+    <t>tab</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>Mason-Dixon Polling</t>
+  </si>
+  <si>
+    <t>Structured survey questions and answers</t>
+  </si>
+  <si>
+    <t>polls</t>
+  </si>
+  <si>
+    <t>questions</t>
+  </si>
+  <si>
+    <t>Raw survey questions and answers</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -364,6 +388,12 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -505,7 +535,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -517,6 +547,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="120">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -13063,17 +13094,53 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C8" sqref="A6:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="9" customFormat="1">
+      <c r="A6" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>